<commit_message>
Updates on qualitative analysis of the interviews
</commit_message>
<xml_diff>
--- a/data/experts/qualitative_analysis_data/third_round_chandler/Julianna.xlsx
+++ b/data/experts/qualitative_analysis_data/third_round_chandler/Julianna.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fronchettl\Documents\GitHub\TOCHI-2023\data\experts\qualitative_analysis_data\third_round_chandler\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{732EEB8C-A9B2-4D14-AAC5-EC9C8EE3983B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA230715-280E-4628-913B-4FD991A6FC2D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7913" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="439" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="440" uniqueCount="104">
   <si>
     <t>Paragraphs</t>
   </si>
@@ -332,13 +332,16 @@
   </si>
   <si>
     <t>Proctor: Thank you so much.</t>
+  </si>
+  <si>
+    <t>Could be used for senstitive objects</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -370,6 +373,13 @@
       <color rgb="FF222222"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="5">
@@ -410,7 +420,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -425,6 +435,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1745,7 +1756,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="63" spans="1:25" ht="60" x14ac:dyDescent="0.4">
+    <row r="63" spans="1:25" ht="45" x14ac:dyDescent="0.4">
       <c r="A63" s="4" t="s">
         <v>66</v>
       </c>
@@ -1875,7 +1886,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="89" spans="1:1" ht="60" x14ac:dyDescent="0.4">
+    <row r="89" spans="1:1" ht="45" x14ac:dyDescent="0.4">
       <c r="A89" s="4" t="s">
         <v>94</v>
       </c>
@@ -1961,7 +1972,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:A97">
-    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="Participant">
+    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="Participant">
       <formula>NOT(ISERROR(SEARCH(("Participant"),(A1))))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3041,7 +3052,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="63" spans="1:25" ht="60" x14ac:dyDescent="0.4">
+    <row r="63" spans="1:25" ht="45" x14ac:dyDescent="0.4">
       <c r="A63" s="4" t="s">
         <v>66</v>
       </c>
@@ -3171,7 +3182,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="89" spans="1:1" ht="60" x14ac:dyDescent="0.4">
+    <row r="89" spans="1:1" ht="45" x14ac:dyDescent="0.4">
       <c r="A89" s="4" t="s">
         <v>94</v>
       </c>
@@ -4337,7 +4348,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="63" spans="1:25" ht="60" x14ac:dyDescent="0.4">
+    <row r="63" spans="1:25" ht="45" x14ac:dyDescent="0.4">
       <c r="A63" s="4" t="s">
         <v>66</v>
       </c>
@@ -4467,7 +4478,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="89" spans="1:1" ht="60" x14ac:dyDescent="0.4">
+    <row r="89" spans="1:1" ht="45" x14ac:dyDescent="0.4">
       <c r="A89" s="4" t="s">
         <v>94</v>
       </c>
@@ -4569,7 +4580,9 @@
   </sheetPr>
   <dimension ref="A1:Y97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A81" workbookViewId="0">
+      <selection activeCell="H95" sqref="H95"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
@@ -5586,6 +5599,9 @@
       <c r="B94" s="7" t="s">
         <v>99</v>
       </c>
+      <c r="H94" s="8" t="s">
+        <v>103</v>
+      </c>
     </row>
     <row r="95" spans="1:8" ht="15" x14ac:dyDescent="0.4">
       <c r="A95" s="4" t="s">
@@ -5607,7 +5623,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:A97">
-    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="Participant">
+    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="Participant">
       <formula>NOT(ISERROR(SEARCH(("Participant"),(A1))))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>